<commit_message>
Adding Array & LinkedList Module
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/AutomationTestData.xlsx
+++ b/src/test/resources/TestData/AutomationTestData.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26124"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venmeen/eclipse-workspace/CucumberNew/src/test/resources/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahaj\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FEB874-F1CF-4741-A5ED-367425950900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pythonCode" sheetId="1" r:id="rId1"/>
+    <sheet name="codeInvalid" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,12 +26,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>pythonCode_valid</t>
-  </si>
-  <si>
-    <t>pythonCode_invalid</t>
   </si>
   <si>
     <t>colors=["red","blue","yellow"] 
@@ -41,11 +40,17 @@
   <si>
     <t>Test</t>
   </si>
+  <si>
+    <t>inValid_pythonCode</t>
+  </si>
+  <si>
+    <t>color = red blue yellow print colors</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -109,6 +114,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -376,34 +384,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850C79A7-E93E-4EE6-AEFD-379F6260D8B5}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="80" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>